<commit_message>
Enable the functionality for 15 PCS panels.
</commit_message>
<xml_diff>
--- a/Application/TouchGFX/assets/texts/texts.xlsx
+++ b/Application/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="117">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -171,6 +171,201 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId51</t>
   </si>
 </sst>
 </file>
@@ -1639,7 +1834,7 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
@@ -1651,12 +1846,12 @@
         <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
@@ -1668,12 +1863,12 @@
         <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
@@ -1685,12 +1880,12 @@
         <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
@@ -1702,7 +1897,704 @@
         <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" t="s">
+        <v>44</v>
+      </c>
+      <c r="F44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added firmware version string to the first screen.
</commit_message>
<xml_diff>
--- a/Application/TouchGFX/assets/texts/texts.xlsx
+++ b/Application/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1835" uniqueCount="122">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -366,6 +366,21 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FW 01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F/W 01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F/W &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId53</t>
   </si>
 </sst>
 </file>
@@ -2597,6 +2612,40 @@
         <v>88</v>
       </c>
     </row>
+    <row r="49">
+      <c r="B49" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>